<commit_message>
IN-1177 fix conflicts again
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF51235-AE82-654F-87C9-3B4E65D3E5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E24F9C5-94DD-AB4C-8298-BDC9CAC0FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8660" yWindow="9140" windowWidth="40920" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2701,7 +2701,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2711,7 +2711,7 @@
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="37.5" customWidth="1"/>
+    <col min="6" max="6" width="45.1640625" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>

</xml_diff>